<commit_message>
Statistical analisys and databases
database constructions  and First statistical analisys.

- Pre IT and IT means and volatility checks (1988 - 2021)
</commit_message>
<xml_diff>
--- a/data/description.xlsx
+++ b/data/description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\00-MQE-UCLA\Capstone\GARCH-CODES\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D01B4804-EBD6-405F-B81F-F621C70EDB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DAF421-D5B4-44F3-8EAD-847937F630A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE28E4E5-3BF4-4F09-887F-28E76258EA44}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve"> cpi</t>
   </si>
@@ -44,30 +44,18 @@
     <t>INE</t>
   </si>
   <si>
-    <t>cpi_total</t>
-  </si>
-  <si>
-    <t>cpi_star</t>
-  </si>
-  <si>
     <t>CPI for All Urban Consumers (CPI-U)</t>
   </si>
   <si>
     <t>U.S. Bureau Of Labor Statistics</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>Tasa de Interés Líder de Polítca Monetaria</t>
   </si>
   <si>
     <t>Banco de Guatemala</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Tipo de Cambio Nominal</t>
   </si>
   <si>
@@ -78,16 +66,61 @@
   </si>
   <si>
     <t>Detalle</t>
+  </si>
+  <si>
+    <t>cpi_usa</t>
+  </si>
+  <si>
+    <t>i_pm</t>
+  </si>
+  <si>
+    <t>ner_gt</t>
+  </si>
+  <si>
+    <t>pce_us</t>
+  </si>
+  <si>
+    <t>pce_us_core</t>
+  </si>
+  <si>
+    <t>imae_tc</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>PCE Inflation USA</t>
+  </si>
+  <si>
+    <t>PCE core inflation USA</t>
+  </si>
+  <si>
+    <t>IMAE gt</t>
+  </si>
+  <si>
+    <t>01/01/2001 - 01/04/2022</t>
+  </si>
+  <si>
+    <t>01/01/1995 - 01/03/2022</t>
+  </si>
+  <si>
+    <t>01/01/1995 -01/04/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,30 +462,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDA14CD-E4F8-48A2-B6F9-2F32C8E22AD3}">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -462,21 +499,27 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -484,30 +527,68 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>